<commit_message>
Continued work on FSK report. Almost done, just need conclusion.
</commit_message>
<xml_diff>
--- a/project/FSK/measurements/Fin to Vout.xlsx
+++ b/project/FSK/measurements/Fin to Vout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15240" tabRatio="500"/>
+    <workbookView xWindow="-19460" yWindow="21600" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,6 +92,30 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Frequency Input</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Vs. Voltage Output</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -101,6 +125,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>2.4GHz Output</c:v>
+          </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -313,6 +340,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>2.6GHz Output</c:v>
+          </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -556,6 +586,25 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frequency (MHz)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
@@ -572,6 +621,25 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Output (V)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -602,16 +670,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -957,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>